<commit_message>
structure-books の更新 ・Youtube-id 列の説明を修正
</commit_message>
<xml_diff>
--- a/chiloPro/sample-series/structure-books_sample.xlsx
+++ b/chiloPro/sample-series/structure-books_sample.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17730" windowHeight="8175"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17730" windowHeight="8175" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="series-information" sheetId="37" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="199">
   <si>
     <t>cover</t>
     <phoneticPr fontId="3"/>
@@ -371,14 +371,6 @@
     </rPh>
     <rPh sb="11" eb="12">
       <t>メイ</t>
-    </rPh>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <t>解説ビデオのYoutubeID
-─────</t>
-    <rPh sb="0" eb="2">
-      <t>カイセツ</t>
     </rPh>
     <phoneticPr fontId="3"/>
   </si>
@@ -1246,6 +1238,40 @@
   </si>
   <si>
     <t>001_cover_image_1.png</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>解説ビデオのYoutubeID
+─────
+Web CHiLO Book用の解説ビデオをYoutubeからビデオを配信する場合、登録したYoutubeビデオのURLに含まれるビデオIDを入力します。
+（例）https://www.youtube.com/watch?v=W6l-nifsu6w　の?v=以降の部分
+注意：入力した場合、ローカル環境からはビデオの再生を確認できません。</t>
+    <rPh sb="64" eb="66">
+      <t>トウロク</t>
+    </rPh>
+    <rPh sb="83" eb="84">
+      <t>フク</t>
+    </rPh>
+    <rPh sb="102" eb="103">
+      <t>レイ</t>
+    </rPh>
+    <rPh sb="152" eb="154">
+      <t>イコウ</t>
+    </rPh>
+    <rPh sb="155" eb="157">
+      <t>ブブン</t>
+    </rPh>
+    <rPh sb="166" eb="168">
+      <t>バアイ</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>解説ビデオのYoutubeID
+─────
+Web CHiLO Book用の解説ビデオをYoutubeから配信する場合、登録したYoutubeビデオのURLに含まれるビデオIDを入力します。
+（例）https://www.youtube.com/watch?v=W6l-nifsu6w　の?v=以降の部分
+注意：入力した場合、ローカル環境からはビデオの再生を確認できません。</t>
     <phoneticPr fontId="3"/>
   </si>
 </sst>
@@ -1440,7 +1466,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="25">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -1721,15 +1747,6 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="hair">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -1910,7 +1927,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="96">
+  <cellXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2100,18 +2117,6 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="49" fontId="16" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection locked="0"/>
@@ -2226,10 +2231,6 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -2640,7 +2641,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
@@ -2653,188 +2654,188 @@
   <sheetData>
     <row r="1" spans="1:5" ht="14.25">
       <c r="A1" s="42" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B1" s="43">
         <v>1</v>
       </c>
       <c r="C1" s="41" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D1" s="40" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="28.5" hidden="1">
       <c r="A2" s="42" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B2" s="43"/>
       <c r="C2" s="41" t="s">
         <v>38</v>
       </c>
       <c r="D2" s="40" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="42.75" hidden="1">
       <c r="A3" s="42" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B3" s="43"/>
       <c r="C3" s="41" t="s">
         <v>39</v>
       </c>
       <c r="D3" s="40" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="28.5">
       <c r="A4" s="42" t="s">
-        <v>72</v>
-      </c>
-      <c r="B4" s="60" t="s">
-        <v>107</v>
+        <v>71</v>
+      </c>
+      <c r="B4" s="57" t="s">
+        <v>106</v>
       </c>
       <c r="C4" s="41" t="s">
         <v>31</v>
       </c>
       <c r="D4" s="40" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="28.5">
       <c r="A5" s="42" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B5" s="44" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C5" s="41" t="s">
         <v>32</v>
       </c>
       <c r="D5" s="40" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="28.5">
       <c r="A6" s="42" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B6" s="44" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C6" s="41" t="s">
         <v>33</v>
       </c>
       <c r="D6" s="40" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="14.25">
       <c r="A7" s="42" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B7" s="44" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C7" s="41" t="s">
         <v>34</v>
       </c>
       <c r="D7" s="40" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="14.25">
       <c r="A8" s="42" t="s">
+        <v>75</v>
+      </c>
+      <c r="B8" s="43" t="s">
         <v>76</v>
-      </c>
-      <c r="B8" s="43" t="s">
-        <v>77</v>
       </c>
       <c r="C8" s="41" t="s">
         <v>41</v>
       </c>
-      <c r="D8" s="64" t="s">
-        <v>64</v>
+      <c r="D8" s="61" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="13.5" customHeight="1">
       <c r="A9" s="42" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B9" s="43" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C9" s="41" t="s">
         <v>42</v>
       </c>
-      <c r="D9" s="65"/>
+      <c r="D9" s="62"/>
     </row>
     <row r="10" spans="1:5" ht="13.5" customHeight="1">
       <c r="A10" s="42" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B10" s="45">
         <v>41530</v>
       </c>
       <c r="C10" s="41" t="s">
-        <v>195</v>
-      </c>
-      <c r="D10" s="65"/>
+        <v>194</v>
+      </c>
+      <c r="D10" s="62"/>
     </row>
     <row r="11" spans="1:5" ht="13.5" customHeight="1">
       <c r="A11" s="42" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B11" s="43" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C11" s="41" t="s">
         <v>35</v>
       </c>
-      <c r="D11" s="66"/>
+      <c r="D11" s="63"/>
     </row>
     <row r="12" spans="1:5" ht="114">
       <c r="A12" s="42" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B12" s="44" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C12" s="41" t="s">
         <v>36</v>
       </c>
       <c r="D12" s="40" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="142.5">
       <c r="A13" s="42" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B13" s="46" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C13" s="41" t="s">
         <v>37</v>
       </c>
       <c r="D13" s="40" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="28.5">
       <c r="A14" s="42" t="s">
-        <v>82</v>
-      </c>
-      <c r="B14" s="61" t="s">
-        <v>112</v>
+        <v>81</v>
+      </c>
+      <c r="B14" s="58" t="s">
+        <v>111</v>
       </c>
       <c r="C14" s="41" t="s">
         <v>40</v>
       </c>
       <c r="D14" s="40" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="14.25">
@@ -2842,101 +2843,101 @@
         <v>0</v>
       </c>
       <c r="B15" s="43" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C15" s="41" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D15" s="40" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="14.25">
       <c r="A16" s="42" t="s">
+        <v>82</v>
+      </c>
+      <c r="B16" s="43" t="s">
+        <v>113</v>
+      </c>
+      <c r="C16" s="41" t="s">
         <v>83</v>
       </c>
-      <c r="B16" s="43" t="s">
-        <v>114</v>
-      </c>
-      <c r="C16" s="41" t="s">
-        <v>84</v>
-      </c>
-      <c r="D16" s="64" t="s">
-        <v>66</v>
-      </c>
-      <c r="E16" s="76" t="s">
-        <v>106</v>
+      <c r="D16" s="61" t="s">
+        <v>65</v>
+      </c>
+      <c r="E16" s="73" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="13.5" customHeight="1">
       <c r="A17" s="42" t="s">
+        <v>84</v>
+      </c>
+      <c r="B17" s="43" t="s">
+        <v>114</v>
+      </c>
+      <c r="C17" s="41" t="s">
         <v>85</v>
       </c>
-      <c r="B17" s="43" t="s">
-        <v>115</v>
-      </c>
-      <c r="C17" s="41" t="s">
-        <v>86</v>
-      </c>
-      <c r="D17" s="65"/>
-      <c r="E17" s="76"/>
+      <c r="D17" s="62"/>
+      <c r="E17" s="73"/>
     </row>
     <row r="18" spans="1:5" ht="13.5" customHeight="1">
       <c r="A18" s="42" t="s">
+        <v>86</v>
+      </c>
+      <c r="B18" s="43" t="s">
+        <v>115</v>
+      </c>
+      <c r="C18" s="41" t="s">
         <v>87</v>
       </c>
-      <c r="B18" s="43" t="s">
-        <v>116</v>
-      </c>
-      <c r="C18" s="41" t="s">
-        <v>88</v>
-      </c>
-      <c r="D18" s="66"/>
-      <c r="E18" s="76"/>
+      <c r="D18" s="63"/>
+      <c r="E18" s="73"/>
     </row>
     <row r="19" spans="1:5" ht="13.5" customHeight="1">
       <c r="A19" s="42" t="s">
+        <v>88</v>
+      </c>
+      <c r="B19" s="43" t="s">
+        <v>116</v>
+      </c>
+      <c r="C19" s="41" t="s">
         <v>89</v>
       </c>
-      <c r="B19" s="43" t="s">
-        <v>117</v>
-      </c>
-      <c r="C19" s="41" t="s">
-        <v>90</v>
-      </c>
       <c r="D19" s="40" t="s">
-        <v>67</v>
-      </c>
-      <c r="E19" s="76"/>
+        <v>66</v>
+      </c>
+      <c r="E19" s="73"/>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="39" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C20" s="37"/>
       <c r="D20" s="38"/>
     </row>
     <row r="22" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A22" s="67" t="s">
-        <v>103</v>
-      </c>
-      <c r="B22" s="68"/>
-      <c r="C22" s="69"/>
+      <c r="A22" s="64" t="s">
+        <v>102</v>
+      </c>
+      <c r="B22" s="65"/>
+      <c r="C22" s="66"/>
     </row>
     <row r="23" spans="1:5">
-      <c r="A23" s="70"/>
-      <c r="B23" s="71"/>
-      <c r="C23" s="72"/>
+      <c r="A23" s="67"/>
+      <c r="B23" s="68"/>
+      <c r="C23" s="69"/>
     </row>
     <row r="24" spans="1:5">
-      <c r="A24" s="70"/>
-      <c r="B24" s="71"/>
-      <c r="C24" s="72"/>
+      <c r="A24" s="67"/>
+      <c r="B24" s="68"/>
+      <c r="C24" s="69"/>
     </row>
     <row r="25" spans="1:5">
-      <c r="A25" s="73"/>
-      <c r="B25" s="74"/>
-      <c r="C25" s="75"/>
+      <c r="A25" s="70"/>
+      <c r="B25" s="71"/>
+      <c r="C25" s="72"/>
     </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
@@ -2977,7 +2978,7 @@
         <v>17</v>
       </c>
       <c r="B1" s="35" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C1" s="6" t="s">
         <v>24</v>
@@ -2991,19 +2992,19 @@
     </row>
     <row r="2" spans="1:5" ht="57.75" thickTop="1">
       <c r="A2" s="26" t="s">
+        <v>117</v>
+      </c>
+      <c r="B2" s="7" t="s">
         <v>118</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="C2" s="47" t="s">
         <v>119</v>
       </c>
-      <c r="C2" s="47" t="s">
+      <c r="D2" s="13" t="s">
         <v>120</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="E2" s="13" t="s">
         <v>121</v>
-      </c>
-      <c r="E2" s="13" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="47.1" customHeight="1">
@@ -3015,13 +3016,13 @@
     </row>
     <row r="4" spans="1:5" ht="128.25">
       <c r="A4" s="29" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B4" s="29" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C4" s="29" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D4" s="29" t="s">
         <v>45</v>
@@ -3036,7 +3037,7 @@
       <c r="C5" s="55"/>
       <c r="D5" s="55"/>
       <c r="E5" s="56" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -3051,32 +3052,32 @@
     </row>
     <row r="8" spans="1:5" ht="14.25" customHeight="1">
       <c r="A8" s="9"/>
-      <c r="B8" s="77" t="s">
-        <v>102</v>
-      </c>
-      <c r="C8" s="78"/>
-      <c r="D8" s="79"/>
+      <c r="B8" s="74" t="s">
+        <v>101</v>
+      </c>
+      <c r="C8" s="75"/>
+      <c r="D8" s="76"/>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="9"/>
-      <c r="B9" s="80"/>
-      <c r="C9" s="81"/>
-      <c r="D9" s="82"/>
+      <c r="B9" s="77"/>
+      <c r="C9" s="78"/>
+      <c r="D9" s="79"/>
     </row>
     <row r="10" spans="1:5">
-      <c r="B10" s="80"/>
-      <c r="C10" s="81"/>
-      <c r="D10" s="82"/>
+      <c r="B10" s="77"/>
+      <c r="C10" s="78"/>
+      <c r="D10" s="79"/>
     </row>
     <row r="11" spans="1:5">
-      <c r="B11" s="80"/>
-      <c r="C11" s="81"/>
-      <c r="D11" s="82"/>
+      <c r="B11" s="77"/>
+      <c r="C11" s="78"/>
+      <c r="D11" s="79"/>
     </row>
     <row r="12" spans="1:5">
-      <c r="B12" s="83"/>
-      <c r="C12" s="84"/>
-      <c r="D12" s="85"/>
+      <c r="B12" s="80"/>
+      <c r="C12" s="81"/>
+      <c r="D12" s="82"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3100,7 +3101,7 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:K29"/>
+  <dimension ref="A1:K28"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3111,10 +3112,10 @@
     <col min="3" max="3" width="23.125" style="11" customWidth="1"/>
     <col min="4" max="4" width="22.5" style="12" customWidth="1"/>
     <col min="5" max="5" width="40.625" style="11" customWidth="1"/>
-    <col min="6" max="6" width="25.5" style="11" customWidth="1"/>
+    <col min="6" max="6" width="30.625" style="11" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.875" style="11" customWidth="1"/>
     <col min="8" max="8" width="12.5" style="11" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="12" style="11" customWidth="1"/>
+    <col min="9" max="9" width="37.5" style="11" customWidth="1"/>
     <col min="10" max="10" width="17.875" style="11" customWidth="1"/>
     <col min="11" max="11" width="8.875" style="4"/>
     <col min="12" max="16384" width="8.875" style="11"/>
@@ -3157,13 +3158,13 @@
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="33" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B2" s="28"/>
       <c r="C2" s="28"/>
       <c r="D2" s="48"/>
       <c r="E2" s="34" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F2" s="28"/>
       <c r="G2" s="28"/>
@@ -3177,26 +3178,26 @@
         <v>1</v>
       </c>
       <c r="B3" s="16" t="s">
+        <v>122</v>
+      </c>
+      <c r="C3" s="16" t="s">
         <v>123</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="D3" s="59" t="s">
+        <v>191</v>
+      </c>
+      <c r="E3" s="16" t="s">
         <v>124</v>
       </c>
-      <c r="D3" s="62" t="s">
-        <v>192</v>
-      </c>
-      <c r="E3" s="16" t="s">
+      <c r="F3" s="16" t="s">
         <v>125</v>
-      </c>
-      <c r="F3" s="16" t="s">
-        <v>126</v>
       </c>
       <c r="G3" s="16" t="s">
         <v>10</v>
       </c>
       <c r="H3" s="16"/>
       <c r="I3" s="16" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="J3" s="16" t="s">
         <v>11</v>
@@ -3208,26 +3209,26 @@
         <v>1</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C4" s="16" t="s">
+        <v>127</v>
+      </c>
+      <c r="D4" s="59" t="s">
+        <v>191</v>
+      </c>
+      <c r="E4" s="16" t="s">
         <v>128</v>
       </c>
-      <c r="D4" s="62" t="s">
-        <v>192</v>
-      </c>
-      <c r="E4" s="16" t="s">
+      <c r="F4" s="16" t="s">
         <v>129</v>
-      </c>
-      <c r="F4" s="16" t="s">
-        <v>130</v>
       </c>
       <c r="G4" s="16" t="s">
         <v>12</v>
       </c>
       <c r="H4" s="16"/>
       <c r="I4" s="16" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="J4" s="16" t="s">
         <v>11</v>
@@ -3239,26 +3240,26 @@
         <v>1</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C5" s="16" t="s">
+        <v>131</v>
+      </c>
+      <c r="D5" s="59" t="s">
+        <v>191</v>
+      </c>
+      <c r="E5" s="16" t="s">
         <v>132</v>
       </c>
-      <c r="D5" s="62" t="s">
-        <v>192</v>
-      </c>
-      <c r="E5" s="16" t="s">
+      <c r="F5" s="16" t="s">
         <v>133</v>
-      </c>
-      <c r="F5" s="16" t="s">
-        <v>134</v>
       </c>
       <c r="G5" s="16" t="s">
         <v>13</v>
       </c>
       <c r="H5" s="16"/>
       <c r="I5" s="16" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J5" s="16" t="s">
         <v>11</v>
@@ -3270,26 +3271,26 @@
         <v>1</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C6" s="16" t="s">
+        <v>135</v>
+      </c>
+      <c r="D6" s="59" t="s">
+        <v>191</v>
+      </c>
+      <c r="E6" s="16" t="s">
         <v>136</v>
       </c>
-      <c r="D6" s="62" t="s">
-        <v>192</v>
-      </c>
-      <c r="E6" s="16" t="s">
+      <c r="F6" s="16" t="s">
         <v>137</v>
-      </c>
-      <c r="F6" s="16" t="s">
-        <v>138</v>
       </c>
       <c r="G6" s="16" t="s">
         <v>14</v>
       </c>
       <c r="H6" s="16"/>
       <c r="I6" s="16" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="J6" s="16" t="s">
         <v>11</v>
@@ -3301,26 +3302,26 @@
         <v>1</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C7" s="16" t="s">
+        <v>139</v>
+      </c>
+      <c r="D7" s="59" t="s">
+        <v>191</v>
+      </c>
+      <c r="E7" s="16" t="s">
         <v>140</v>
       </c>
-      <c r="D7" s="62" t="s">
-        <v>192</v>
-      </c>
-      <c r="E7" s="16" t="s">
+      <c r="F7" s="16" t="s">
         <v>141</v>
-      </c>
-      <c r="F7" s="16" t="s">
-        <v>142</v>
       </c>
       <c r="G7" s="16" t="s">
         <v>15</v>
       </c>
       <c r="H7" s="16"/>
       <c r="I7" s="16" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="J7" s="16" t="s">
         <v>11</v>
@@ -3332,26 +3333,26 @@
         <v>1</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C8" s="16" t="s">
+        <v>143</v>
+      </c>
+      <c r="D8" s="59" t="s">
+        <v>191</v>
+      </c>
+      <c r="E8" s="16" t="s">
         <v>144</v>
       </c>
-      <c r="D8" s="62" t="s">
-        <v>192</v>
-      </c>
-      <c r="E8" s="16" t="s">
+      <c r="F8" s="16" t="s">
         <v>145</v>
       </c>
-      <c r="F8" s="16" t="s">
+      <c r="G8" s="16" t="s">
         <v>146</v>
-      </c>
-      <c r="G8" s="16" t="s">
-        <v>147</v>
       </c>
       <c r="H8" s="16"/>
       <c r="I8" s="16" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="J8" s="16" t="s">
         <v>11</v>
@@ -3363,26 +3364,26 @@
         <v>1</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C9" s="16" t="s">
+        <v>148</v>
+      </c>
+      <c r="D9" s="59" t="s">
+        <v>191</v>
+      </c>
+      <c r="E9" s="16" t="s">
         <v>149</v>
       </c>
-      <c r="D9" s="62" t="s">
-        <v>192</v>
-      </c>
-      <c r="E9" s="16" t="s">
+      <c r="F9" s="16" t="s">
         <v>150</v>
       </c>
-      <c r="F9" s="16" t="s">
+      <c r="G9" s="16" t="s">
         <v>151</v>
-      </c>
-      <c r="G9" s="16" t="s">
-        <v>152</v>
       </c>
       <c r="H9" s="16"/>
       <c r="I9" s="16" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="J9" s="16" t="s">
         <v>11</v>
@@ -3394,26 +3395,26 @@
         <v>1</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C10" s="16" t="s">
+        <v>153</v>
+      </c>
+      <c r="D10" s="59" t="s">
+        <v>191</v>
+      </c>
+      <c r="E10" s="16" t="s">
         <v>154</v>
       </c>
-      <c r="D10" s="62" t="s">
-        <v>192</v>
-      </c>
-      <c r="E10" s="16" t="s">
+      <c r="F10" s="16" t="s">
         <v>155</v>
       </c>
-      <c r="F10" s="16" t="s">
+      <c r="G10" s="16" t="s">
         <v>156</v>
-      </c>
-      <c r="G10" s="16" t="s">
-        <v>157</v>
       </c>
       <c r="H10" s="16"/>
       <c r="I10" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="J10" s="16" t="s">
         <v>11</v>
@@ -3425,26 +3426,26 @@
         <v>1</v>
       </c>
       <c r="B11" s="16" t="s">
+        <v>158</v>
+      </c>
+      <c r="C11" s="16" t="s">
         <v>159</v>
       </c>
-      <c r="C11" s="16" t="s">
+      <c r="D11" s="59" t="s">
+        <v>191</v>
+      </c>
+      <c r="E11" s="16" t="s">
         <v>160</v>
       </c>
-      <c r="D11" s="62" t="s">
-        <v>192</v>
-      </c>
-      <c r="E11" s="16" t="s">
+      <c r="F11" s="16" t="s">
         <v>161</v>
       </c>
-      <c r="F11" s="16" t="s">
+      <c r="G11" s="16" t="s">
         <v>162</v>
-      </c>
-      <c r="G11" s="16" t="s">
-        <v>163</v>
       </c>
       <c r="H11" s="16"/>
       <c r="I11" s="16" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="J11" s="16" t="s">
         <v>11</v>
@@ -3456,26 +3457,26 @@
         <v>1</v>
       </c>
       <c r="B12" s="16" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C12" s="16" t="s">
+        <v>164</v>
+      </c>
+      <c r="D12" s="59" t="s">
+        <v>191</v>
+      </c>
+      <c r="E12" s="16" t="s">
         <v>165</v>
       </c>
-      <c r="D12" s="62" t="s">
-        <v>192</v>
-      </c>
-      <c r="E12" s="16" t="s">
+      <c r="F12" s="16" t="s">
         <v>166</v>
       </c>
-      <c r="F12" s="16" t="s">
+      <c r="G12" s="16" t="s">
         <v>167</v>
-      </c>
-      <c r="G12" s="16" t="s">
-        <v>168</v>
       </c>
       <c r="H12" s="16"/>
       <c r="I12" s="16" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="J12" s="16" t="s">
         <v>11</v>
@@ -3487,26 +3488,26 @@
         <v>1</v>
       </c>
       <c r="B13" s="16" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C13" s="16" t="s">
+        <v>169</v>
+      </c>
+      <c r="D13" s="59" t="s">
+        <v>191</v>
+      </c>
+      <c r="E13" s="16" t="s">
         <v>170</v>
       </c>
-      <c r="D13" s="62" t="s">
-        <v>192</v>
-      </c>
-      <c r="E13" s="16" t="s">
+      <c r="F13" s="16" t="s">
         <v>171</v>
       </c>
-      <c r="F13" s="16" t="s">
+      <c r="G13" s="16" t="s">
         <v>172</v>
-      </c>
-      <c r="G13" s="16" t="s">
-        <v>173</v>
       </c>
       <c r="H13" s="16"/>
       <c r="I13" s="16" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="J13" s="16" t="s">
         <v>11</v>
@@ -3518,26 +3519,26 @@
         <v>1</v>
       </c>
       <c r="B14" s="16" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C14" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="D14" s="59" t="s">
+        <v>191</v>
+      </c>
+      <c r="E14" s="16" t="s">
         <v>175</v>
       </c>
-      <c r="D14" s="62" t="s">
-        <v>192</v>
-      </c>
-      <c r="E14" s="16" t="s">
+      <c r="F14" s="16" t="s">
         <v>176</v>
       </c>
-      <c r="F14" s="16" t="s">
+      <c r="G14" s="16" t="s">
         <v>177</v>
-      </c>
-      <c r="G14" s="16" t="s">
-        <v>178</v>
       </c>
       <c r="H14" s="16"/>
       <c r="I14" s="16" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="J14" s="16" t="s">
         <v>11</v>
@@ -3549,26 +3550,26 @@
         <v>1</v>
       </c>
       <c r="B15" s="16" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C15" s="16" t="s">
+        <v>179</v>
+      </c>
+      <c r="D15" s="59" t="s">
+        <v>191</v>
+      </c>
+      <c r="E15" s="16" t="s">
         <v>180</v>
       </c>
-      <c r="D15" s="62" t="s">
-        <v>192</v>
-      </c>
-      <c r="E15" s="16" t="s">
+      <c r="F15" s="16" t="s">
         <v>181</v>
       </c>
-      <c r="F15" s="16" t="s">
+      <c r="G15" s="16" t="s">
         <v>182</v>
-      </c>
-      <c r="G15" s="16" t="s">
-        <v>183</v>
       </c>
       <c r="H15" s="16"/>
       <c r="I15" s="16" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="J15" s="16" t="s">
         <v>11</v>
@@ -3580,26 +3581,26 @@
         <v>1</v>
       </c>
       <c r="B16" s="16" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C16" s="16" t="s">
+        <v>184</v>
+      </c>
+      <c r="D16" s="59" t="s">
+        <v>191</v>
+      </c>
+      <c r="E16" s="16" t="s">
         <v>185</v>
       </c>
-      <c r="D16" s="62" t="s">
-        <v>192</v>
-      </c>
-      <c r="E16" s="16" t="s">
+      <c r="F16" s="16" t="s">
         <v>186</v>
       </c>
-      <c r="F16" s="16" t="s">
+      <c r="G16" s="16" t="s">
         <v>187</v>
-      </c>
-      <c r="G16" s="16" t="s">
-        <v>188</v>
       </c>
       <c r="H16" s="16"/>
       <c r="I16" s="16" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="J16" s="16" t="s">
         <v>11</v>
@@ -3611,12 +3612,12 @@
         <v>16</v>
       </c>
       <c r="B17" s="16" t="s">
+        <v>189</v>
+      </c>
+      <c r="C17" s="16"/>
+      <c r="D17" s="59"/>
+      <c r="E17" s="17" t="s">
         <v>190</v>
-      </c>
-      <c r="C17" s="16"/>
-      <c r="D17" s="62"/>
-      <c r="E17" s="17" t="s">
-        <v>191</v>
       </c>
       <c r="F17" s="16"/>
       <c r="G17" s="16"/>
@@ -3640,7 +3641,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="19" spans="1:11" s="53" customFormat="1" ht="108">
+    <row r="19" spans="1:11" s="53" customFormat="1" ht="148.5">
       <c r="A19" s="50" t="s">
         <v>47</v>
       </c>
@@ -3654,7 +3655,7 @@
         <v>50</v>
       </c>
       <c r="E19" s="50" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F19" s="50" t="s">
         <v>51</v>
@@ -3663,63 +3664,61 @@
         <v>52</v>
       </c>
       <c r="H19" s="50" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I19" s="50" t="s">
+        <v>197</v>
+      </c>
+      <c r="J19" s="50" t="s">
         <v>53</v>
       </c>
-      <c r="J19" s="50" t="s">
-        <v>54</v>
-      </c>
       <c r="K19" s="52"/>
     </row>
-    <row r="20" spans="1:11" s="57" customFormat="1" ht="36" customHeight="1">
-      <c r="D20" s="58"/>
-      <c r="I20" s="95" t="s">
-        <v>106</v>
-      </c>
-      <c r="J20" s="95"/>
-      <c r="K20" s="59"/>
+    <row r="20" spans="1:11" s="21" customFormat="1">
+      <c r="D20" s="22"/>
+      <c r="K20" s="23"/>
     </row>
     <row r="21" spans="1:11" s="21" customFormat="1">
       <c r="D21" s="22"/>
       <c r="K21" s="23"/>
     </row>
-    <row r="22" spans="1:11" s="21" customFormat="1">
-      <c r="D22" s="22"/>
-      <c r="K22" s="23"/>
-    </row>
-    <row r="23" spans="1:11" ht="14.25" customHeight="1">
-      <c r="B23" s="86" t="s">
-        <v>101</v>
-      </c>
+    <row r="22" spans="1:11" ht="14.25" customHeight="1">
+      <c r="B22" s="83" t="s">
+        <v>100</v>
+      </c>
+      <c r="C22" s="84"/>
+      <c r="D22" s="84"/>
+      <c r="E22" s="85"/>
+    </row>
+    <row r="23" spans="1:11">
+      <c r="B23" s="86"/>
       <c r="C23" s="87"/>
       <c r="D23" s="87"/>
       <c r="E23" s="88"/>
     </row>
     <row r="24" spans="1:11">
-      <c r="B24" s="89"/>
-      <c r="C24" s="90"/>
-      <c r="D24" s="90"/>
-      <c r="E24" s="91"/>
+      <c r="B24" s="86"/>
+      <c r="C24" s="87"/>
+      <c r="D24" s="87"/>
+      <c r="E24" s="88"/>
     </row>
     <row r="25" spans="1:11">
-      <c r="B25" s="89"/>
-      <c r="C25" s="90"/>
-      <c r="D25" s="90"/>
-      <c r="E25" s="91"/>
+      <c r="B25" s="86"/>
+      <c r="C25" s="87"/>
+      <c r="D25" s="87"/>
+      <c r="E25" s="88"/>
     </row>
     <row r="26" spans="1:11">
-      <c r="B26" s="89"/>
-      <c r="C26" s="90"/>
-      <c r="D26" s="90"/>
-      <c r="E26" s="91"/>
+      <c r="B26" s="86"/>
+      <c r="C26" s="87"/>
+      <c r="D26" s="87"/>
+      <c r="E26" s="88"/>
     </row>
     <row r="27" spans="1:11">
-      <c r="B27" s="89"/>
-      <c r="C27" s="90"/>
-      <c r="D27" s="90"/>
-      <c r="E27" s="91"/>
+      <c r="B27" s="86"/>
+      <c r="C27" s="87"/>
+      <c r="D27" s="87"/>
+      <c r="E27" s="88"/>
     </row>
     <row r="28" spans="1:11">
       <c r="B28" s="89"/>
@@ -3727,17 +3726,10 @@
       <c r="D28" s="90"/>
       <c r="E28" s="91"/>
     </row>
-    <row r="29" spans="1:11">
-      <c r="B29" s="92"/>
-      <c r="C29" s="93"/>
-      <c r="D29" s="93"/>
-      <c r="E29" s="94"/>
-    </row>
   </sheetData>
-  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
-  <mergeCells count="2">
-    <mergeCell ref="B23:E29"/>
-    <mergeCell ref="I20:J20"/>
+  <sheetProtection sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
+  <mergeCells count="1">
+    <mergeCell ref="B22:E28"/>
   </mergeCells>
   <phoneticPr fontId="3"/>
   <hyperlinks>
@@ -3778,9 +3770,9 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet4"/>
-  <dimension ref="A1:K24"/>
+  <dimension ref="A1:K23"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25"/>
   <cols>
@@ -3792,7 +3784,7 @@
     <col min="6" max="6" width="25.5" style="11" customWidth="1"/>
     <col min="7" max="7" width="13.875" style="11" customWidth="1"/>
     <col min="8" max="8" width="12.5" style="11" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="12" style="11" customWidth="1"/>
+    <col min="9" max="9" width="37.5" style="11" customWidth="1"/>
     <col min="10" max="10" width="17.875" style="11" customWidth="1"/>
     <col min="11" max="11" width="8.875" style="4"/>
     <col min="12" max="16384" width="8.875" style="11"/>
@@ -3841,7 +3833,7 @@
       <c r="C2" s="28"/>
       <c r="D2" s="48"/>
       <c r="E2" s="34" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F2" s="28"/>
       <c r="G2" s="28"/>
@@ -3987,7 +3979,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="1:11" s="53" customFormat="1" ht="108">
+    <row r="14" spans="1:11" s="53" customFormat="1" ht="148.5">
       <c r="A14" s="50" t="s">
         <v>47</v>
       </c>
@@ -4001,7 +3993,7 @@
         <v>50</v>
       </c>
       <c r="E14" s="50" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F14" s="50" t="s">
         <v>51</v>
@@ -4010,81 +4002,72 @@
         <v>52</v>
       </c>
       <c r="H14" s="50" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I14" s="50" t="s">
+        <v>198</v>
+      </c>
+      <c r="J14" s="50" t="s">
         <v>53</v>
       </c>
-      <c r="J14" s="50" t="s">
-        <v>54</v>
-      </c>
       <c r="K14" s="52"/>
     </row>
-    <row r="15" spans="1:11" s="57" customFormat="1" ht="36" customHeight="1">
-      <c r="D15" s="58"/>
-      <c r="I15" s="95" t="s">
-        <v>106</v>
-      </c>
-      <c r="J15" s="95"/>
-      <c r="K15" s="59"/>
+    <row r="15" spans="1:11" s="21" customFormat="1">
+      <c r="D15" s="22"/>
+      <c r="K15" s="23"/>
     </row>
     <row r="16" spans="1:11" s="21" customFormat="1">
       <c r="D16" s="22"/>
       <c r="K16" s="23"/>
     </row>
-    <row r="17" spans="2:11" s="21" customFormat="1">
-      <c r="D17" s="22"/>
-      <c r="K17" s="23"/>
-    </row>
-    <row r="18" spans="2:11" ht="14.25" customHeight="1">
-      <c r="B18" s="86" t="s">
-        <v>101</v>
-      </c>
+    <row r="17" spans="2:5" ht="14.25" customHeight="1">
+      <c r="B17" s="83" t="s">
+        <v>100</v>
+      </c>
+      <c r="C17" s="84"/>
+      <c r="D17" s="84"/>
+      <c r="E17" s="85"/>
+    </row>
+    <row r="18" spans="2:5">
+      <c r="B18" s="86"/>
       <c r="C18" s="87"/>
       <c r="D18" s="87"/>
       <c r="E18" s="88"/>
     </row>
-    <row r="19" spans="2:11">
-      <c r="B19" s="89"/>
-      <c r="C19" s="90"/>
-      <c r="D19" s="90"/>
-      <c r="E19" s="91"/>
-    </row>
-    <row r="20" spans="2:11">
-      <c r="B20" s="89"/>
-      <c r="C20" s="90"/>
-      <c r="D20" s="90"/>
-      <c r="E20" s="91"/>
-    </row>
-    <row r="21" spans="2:11">
-      <c r="B21" s="89"/>
-      <c r="C21" s="90"/>
-      <c r="D21" s="90"/>
-      <c r="E21" s="91"/>
-    </row>
-    <row r="22" spans="2:11">
-      <c r="B22" s="89"/>
-      <c r="C22" s="90"/>
-      <c r="D22" s="90"/>
-      <c r="E22" s="91"/>
-    </row>
-    <row r="23" spans="2:11">
+    <row r="19" spans="2:5">
+      <c r="B19" s="86"/>
+      <c r="C19" s="87"/>
+      <c r="D19" s="87"/>
+      <c r="E19" s="88"/>
+    </row>
+    <row r="20" spans="2:5">
+      <c r="B20" s="86"/>
+      <c r="C20" s="87"/>
+      <c r="D20" s="87"/>
+      <c r="E20" s="88"/>
+    </row>
+    <row r="21" spans="2:5">
+      <c r="B21" s="86"/>
+      <c r="C21" s="87"/>
+      <c r="D21" s="87"/>
+      <c r="E21" s="88"/>
+    </row>
+    <row r="22" spans="2:5">
+      <c r="B22" s="86"/>
+      <c r="C22" s="87"/>
+      <c r="D22" s="87"/>
+      <c r="E22" s="88"/>
+    </row>
+    <row r="23" spans="2:5">
       <c r="B23" s="89"/>
       <c r="C23" s="90"/>
       <c r="D23" s="90"/>
       <c r="E23" s="91"/>
     </row>
-    <row r="24" spans="2:11">
-      <c r="B24" s="92"/>
-      <c r="C24" s="93"/>
-      <c r="D24" s="93"/>
-      <c r="E24" s="94"/>
-    </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
-  <mergeCells count="2">
-    <mergeCell ref="I15:J15"/>
-    <mergeCell ref="B18:E24"/>
+  <sheetProtection sheet="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
+  <mergeCells count="1">
+    <mergeCell ref="B17:E23"/>
   </mergeCells>
   <phoneticPr fontId="3"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4143,8 +4126,8 @@
       <c r="A2" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="63" t="s">
-        <v>193</v>
+      <c r="B2" s="60" t="s">
+        <v>192</v>
       </c>
       <c r="C2" s="19" t="s">
         <v>11</v>
@@ -4152,7 +4135,7 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="18" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B3" s="18"/>
       <c r="C3" s="18" t="s">

</xml_diff>

<commit_message>
項目名の変更　section, page -> chapter, section
</commit_message>
<xml_diff>
--- a/chiloPro/sample-series/structure-books_sample.xlsx
+++ b/chiloPro/sample-series/structure-books_sample.xlsx
@@ -43,9 +43,6 @@
     <t>epub-download-url</t>
   </si>
   <si>
-    <t>page</t>
-  </si>
-  <si>
     <t>main</t>
   </si>
   <si>
@@ -94,16 +91,6 @@
   <si>
     <t>page-type（必須）</t>
     <rPh sb="10" eb="12">
-      <t>ヒッス</t>
-    </rPh>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <t>section（B2以降必須）</t>
-    <rPh sb="10" eb="12">
-      <t>イコウ</t>
-    </rPh>
-    <rPh sb="12" eb="14">
       <t>ヒッス</t>
     </rPh>
     <phoneticPr fontId="3"/>
@@ -278,23 +265,6 @@
 test…テストページ</t>
     <rPh sb="31" eb="33">
       <t>カイセツ</t>
-    </rPh>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <t>セクションタイトル
-────────</t>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <t>ページタイトル
-───────
-page-typeがtestの場合は記載する必要がありません</t>
-    <rPh sb="34" eb="36">
-      <t>キサイ</t>
-    </rPh>
-    <rPh sb="38" eb="40">
-      <t>ヒツヨウ</t>
     </rPh>
     <phoneticPr fontId="3"/>
   </si>
@@ -1221,6 +1191,29 @@
     </rPh>
     <rPh sb="3" eb="6">
       <t>ハッコウビ</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>chapter（B2以降必須）</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>section</t>
+  </si>
+  <si>
+    <t>チャプタータイトル
+────────</t>
+  </si>
+  <si>
+    <t>セクションタイトル
+───────
+page-typeがtestの場合は記載する必要がありません</t>
+    <rPh sb="36" eb="38">
+      <t>キサイ</t>
+    </rPh>
+    <rPh sb="40" eb="42">
+      <t>ヒツヨウ</t>
     </rPh>
     <phoneticPr fontId="3"/>
   </si>
@@ -2602,148 +2595,148 @@
   <sheetData>
     <row r="1" spans="1:5" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A1" s="33" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B1" s="34">
         <v>1</v>
       </c>
       <c r="C1" s="32" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D1" s="31" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="28.5" x14ac:dyDescent="0.15">
       <c r="A2" s="33" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B2" s="35" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C2" s="32" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D2" s="31" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A3" s="33" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B3" s="35" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C3" s="32" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D3" s="31" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A4" s="33" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B4" s="34" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C4" s="32" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D4" s="64" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="33" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B5" s="34" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C5" s="32" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D5" s="65"/>
     </row>
     <row r="6" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="33" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B6" s="61">
         <v>41530</v>
       </c>
       <c r="C6" s="32" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="D6" s="65"/>
     </row>
     <row r="7" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="33" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="B7" s="36">
         <v>42094</v>
       </c>
       <c r="C7" s="32" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="D7" s="65"/>
     </row>
     <row r="8" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="33" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B8" s="34" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C8" s="32" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D8" s="66"/>
     </row>
     <row r="9" spans="1:5" ht="114" x14ac:dyDescent="0.15">
       <c r="A9" s="33" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B9" s="35" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C9" s="32" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D9" s="31" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="142.5" x14ac:dyDescent="0.15">
       <c r="A10" s="33" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B10" s="37" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C10" s="32" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D10" s="31" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="28.5" x14ac:dyDescent="0.15">
       <c r="A11" s="33" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B11" s="47" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="C11" s="32" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D11" s="31" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="14.25" x14ac:dyDescent="0.15">
@@ -2751,98 +2744,98 @@
         <v>0</v>
       </c>
       <c r="B12" s="34" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="C12" s="32" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D12" s="31" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A13" s="33" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="B13" s="47" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="C13" s="32" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="D13" s="50" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="E13" s="76" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A14" s="33" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B14" s="34" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C14" s="32" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="D14" s="64" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="E14" s="76"/>
     </row>
     <row r="15" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="33" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B15" s="46" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C15" s="32" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="D15" s="65"/>
       <c r="E15" s="76"/>
     </row>
     <row r="16" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="33" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B16" s="34" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="C16" s="32" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="D16" s="66"/>
       <c r="E16" s="76"/>
     </row>
     <row r="17" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="33" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B17" s="34" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="C17" s="32" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="D17" s="31" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="E17" s="76"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A18" s="30" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C18" s="28"/>
       <c r="D18" s="29"/>
     </row>
     <row r="20" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="67" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B20" s="68"/>
       <c r="C20" s="69"/>
@@ -2901,22 +2894,22 @@
   <sheetData>
     <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B1" s="26" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C1" s="52" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D1" s="26" t="s">
+        <v>182</v>
+      </c>
+      <c r="E1" s="26" t="s">
         <v>186</v>
       </c>
-      <c r="E1" s="26" t="s">
-        <v>190</v>
-      </c>
       <c r="F1" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G1" s="5" t="s">
         <v>2</v>
@@ -2924,25 +2917,25 @@
     </row>
     <row r="2" spans="1:7" ht="57.75" thickTop="1" x14ac:dyDescent="0.15">
       <c r="A2" s="56" t="s">
+        <v>94</v>
+      </c>
+      <c r="B2" s="57" t="s">
+        <v>95</v>
+      </c>
+      <c r="C2" s="53" t="s">
+        <v>96</v>
+      </c>
+      <c r="D2" s="51" t="s">
+        <v>184</v>
+      </c>
+      <c r="E2" s="62" t="s">
+        <v>181</v>
+      </c>
+      <c r="F2" s="58" t="s">
+        <v>97</v>
+      </c>
+      <c r="G2" s="58" t="s">
         <v>98</v>
-      </c>
-      <c r="B2" s="57" t="s">
-        <v>99</v>
-      </c>
-      <c r="C2" s="53" t="s">
-        <v>100</v>
-      </c>
-      <c r="D2" s="51" t="s">
-        <v>188</v>
-      </c>
-      <c r="E2" s="62" t="s">
-        <v>185</v>
-      </c>
-      <c r="F2" s="58" t="s">
-        <v>101</v>
-      </c>
-      <c r="G2" s="58" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="47.1" customHeight="1" x14ac:dyDescent="0.15">
@@ -2956,25 +2949,25 @@
     </row>
     <row r="4" spans="1:7" ht="128.25" x14ac:dyDescent="0.15">
       <c r="A4" s="22" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B4" s="22" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C4" s="22" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="D4" s="22" t="s">
+        <v>183</v>
+      </c>
+      <c r="E4" s="22" t="s">
         <v>187</v>
       </c>
-      <c r="E4" s="22" t="s">
-        <v>191</v>
-      </c>
       <c r="F4" s="22" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G4" s="22" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="28.5" x14ac:dyDescent="0.15">
@@ -2984,7 +2977,7 @@
       <c r="D5" s="44"/>
       <c r="F5" s="44"/>
       <c r="G5" s="45" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.15">
@@ -3001,7 +2994,7 @@
     <row r="8" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="6"/>
       <c r="B8" s="77" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C8" s="78"/>
       <c r="D8" s="79"/>
@@ -3060,7 +3053,9 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:K27"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
   <cols>
@@ -3080,37 +3075,37 @@
   <sheetData>
     <row r="1" spans="1:11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>19</v>
+        <v>190</v>
       </c>
       <c r="C1" s="11" t="s">
+        <v>191</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="E1" s="11" t="s">
+      <c r="F1" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="G1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="H1" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="I1" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="J1" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="11" t="s">
-        <v>9</v>
-      </c>
       <c r="K1" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.15">
@@ -3118,29 +3113,29 @@
         <v>1</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="D2" s="48" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H2" s="12"/>
       <c r="I2" s="12" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="J2" s="12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K2" s="10"/>
     </row>
@@ -3149,29 +3144,29 @@
         <v>1</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="D3" s="48" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="F3" s="12" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="G3" s="12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H3" s="12"/>
       <c r="I3" s="12" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="J3" s="12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K3" s="10"/>
     </row>
@@ -3180,29 +3175,29 @@
         <v>1</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="D4" s="48" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="G4" s="12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H4" s="12"/>
       <c r="I4" s="12" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="J4" s="12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K4" s="10"/>
     </row>
@@ -3211,29 +3206,29 @@
         <v>1</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="D5" s="48" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="G5" s="12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H5" s="12"/>
       <c r="I5" s="12" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="J5" s="12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K5" s="10"/>
     </row>
@@ -3242,29 +3237,29 @@
         <v>1</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="D6" s="48" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="G6" s="12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H6" s="12"/>
       <c r="I6" s="12" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="J6" s="12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K6" s="10"/>
     </row>
@@ -3273,29 +3268,29 @@
         <v>1</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="D7" s="48" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="G7" s="12" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="H7" s="12"/>
       <c r="I7" s="12" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="J7" s="12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K7" s="10"/>
     </row>
@@ -3304,29 +3299,29 @@
         <v>1</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="D8" s="48" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="F8" s="12" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="G8" s="12" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="H8" s="12"/>
       <c r="I8" s="12" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="J8" s="12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K8" s="10"/>
     </row>
@@ -3335,29 +3330,29 @@
         <v>1</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="D9" s="48" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="F9" s="12" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="G9" s="12" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="H9" s="12"/>
       <c r="I9" s="12" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="J9" s="12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K9" s="10"/>
     </row>
@@ -3366,29 +3361,29 @@
         <v>1</v>
       </c>
       <c r="B10" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="D10" s="48" t="s">
+        <v>167</v>
+      </c>
+      <c r="E10" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>138</v>
+      </c>
+      <c r="G10" s="12" t="s">
         <v>139</v>
-      </c>
-      <c r="C10" s="12" t="s">
-        <v>140</v>
-      </c>
-      <c r="D10" s="48" t="s">
-        <v>171</v>
-      </c>
-      <c r="E10" s="12" t="s">
-        <v>141</v>
-      </c>
-      <c r="F10" s="12" t="s">
-        <v>142</v>
-      </c>
-      <c r="G10" s="12" t="s">
-        <v>143</v>
       </c>
       <c r="H10" s="12"/>
       <c r="I10" s="12" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="J10" s="12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K10" s="10"/>
     </row>
@@ -3397,29 +3392,29 @@
         <v>1</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="D11" s="48" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="F11" s="12" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="G11" s="12" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="H11" s="12"/>
       <c r="I11" s="12" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="J11" s="12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K11" s="10"/>
     </row>
@@ -3428,29 +3423,29 @@
         <v>1</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="D12" s="48" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="F12" s="12" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="G12" s="12" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="H12" s="12"/>
       <c r="I12" s="12" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="J12" s="12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K12" s="10"/>
     </row>
@@ -3459,29 +3454,29 @@
         <v>1</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="D13" s="48" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="F13" s="12" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="G13" s="12" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="H13" s="12"/>
       <c r="I13" s="12" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="J13" s="12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K13" s="10"/>
     </row>
@@ -3490,29 +3485,29 @@
         <v>1</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="D14" s="48" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="F14" s="12" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="G14" s="12" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="H14" s="12"/>
       <c r="I14" s="12" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="J14" s="12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K14" s="10"/>
     </row>
@@ -3521,43 +3516,43 @@
         <v>1</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="D15" s="48" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="F15" s="12" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="G15" s="12" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="H15" s="12"/>
       <c r="I15" s="12" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="J15" s="12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K15" s="10"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A16" s="12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="C16" s="12"/>
       <c r="D16" s="48"/>
       <c r="E16" s="13" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="F16" s="12"/>
       <c r="G16" s="12"/>
@@ -3578,39 +3573,39 @@
       <c r="I17" s="24"/>
       <c r="J17" s="24"/>
       <c r="K17" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="18" spans="1:11" s="42" customFormat="1" ht="148.5" x14ac:dyDescent="0.15">
       <c r="A18" s="39" t="s">
+        <v>41</v>
+      </c>
+      <c r="B18" s="39" t="s">
+        <v>192</v>
+      </c>
+      <c r="C18" s="39" t="s">
+        <v>193</v>
+      </c>
+      <c r="D18" s="40" t="s">
+        <v>42</v>
+      </c>
+      <c r="E18" s="39" t="s">
+        <v>83</v>
+      </c>
+      <c r="F18" s="39" t="s">
         <v>43</v>
       </c>
-      <c r="B18" s="39" t="s">
+      <c r="G18" s="39" t="s">
         <v>44</v>
       </c>
-      <c r="C18" s="39" t="s">
+      <c r="H18" s="39" t="s">
+        <v>48</v>
+      </c>
+      <c r="I18" s="39" t="s">
+        <v>170</v>
+      </c>
+      <c r="J18" s="39" t="s">
         <v>45</v>
-      </c>
-      <c r="D18" s="40" t="s">
-        <v>46</v>
-      </c>
-      <c r="E18" s="39" t="s">
-        <v>87</v>
-      </c>
-      <c r="F18" s="39" t="s">
-        <v>47</v>
-      </c>
-      <c r="G18" s="39" t="s">
-        <v>48</v>
-      </c>
-      <c r="H18" s="39" t="s">
-        <v>52</v>
-      </c>
-      <c r="I18" s="39" t="s">
-        <v>174</v>
-      </c>
-      <c r="J18" s="39" t="s">
-        <v>49</v>
       </c>
       <c r="K18" s="41"/>
     </row>
@@ -3624,7 +3619,7 @@
     </row>
     <row r="21" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B21" s="86" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C21" s="87"/>
       <c r="D21" s="87"/>
@@ -3732,37 +3727,37 @@
   <sheetData>
     <row r="1" spans="1:11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>19</v>
+        <v>190</v>
       </c>
       <c r="C1" s="11" t="s">
+        <v>191</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="E1" s="11" t="s">
+      <c r="F1" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="G1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="H1" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="I1" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="J1" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="11" t="s">
-        <v>9</v>
-      </c>
       <c r="K1" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.15">
@@ -3899,39 +3894,39 @@
       <c r="I12" s="24"/>
       <c r="J12" s="24"/>
       <c r="K12" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:11" s="42" customFormat="1" ht="148.5" x14ac:dyDescent="0.15">
       <c r="A13" s="39" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13" s="39" t="s">
+        <v>192</v>
+      </c>
+      <c r="C13" s="39" t="s">
+        <v>193</v>
+      </c>
+      <c r="D13" s="40" t="s">
+        <v>42</v>
+      </c>
+      <c r="E13" s="39" t="s">
+        <v>83</v>
+      </c>
+      <c r="F13" s="39" t="s">
         <v>43</v>
       </c>
-      <c r="B13" s="39" t="s">
+      <c r="G13" s="39" t="s">
         <v>44</v>
       </c>
-      <c r="C13" s="39" t="s">
+      <c r="H13" s="39" t="s">
+        <v>48</v>
+      </c>
+      <c r="I13" s="39" t="s">
+        <v>171</v>
+      </c>
+      <c r="J13" s="39" t="s">
         <v>45</v>
-      </c>
-      <c r="D13" s="40" t="s">
-        <v>46</v>
-      </c>
-      <c r="E13" s="39" t="s">
-        <v>87</v>
-      </c>
-      <c r="F13" s="39" t="s">
-        <v>47</v>
-      </c>
-      <c r="G13" s="39" t="s">
-        <v>48</v>
-      </c>
-      <c r="H13" s="39" t="s">
-        <v>52</v>
-      </c>
-      <c r="I13" s="39" t="s">
-        <v>175</v>
-      </c>
-      <c r="J13" s="39" t="s">
-        <v>49</v>
       </c>
       <c r="K13" s="41"/>
     </row>
@@ -3945,7 +3940,7 @@
     </row>
     <row r="16" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B16" s="86" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C16" s="87"/>
       <c r="D16" s="87"/>
@@ -4038,61 +4033,61 @@
   <sheetData>
     <row r="1" spans="1:3" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A1" s="16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="14.25" thickTop="1" x14ac:dyDescent="0.15">
       <c r="A2" s="15" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B2" s="49" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A3" s="14" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="B3" s="14"/>
       <c r="C3" s="14" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A4" s="14"/>
       <c r="B4" s="14"/>
       <c r="C4" s="14" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A5" s="14"/>
       <c r="B5" s="14"/>
       <c r="C5" s="14" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A6" s="14"/>
       <c r="B6" s="14"/>
       <c r="C6" s="14" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A7" s="14"/>
       <c r="B7" s="14"/>
       <c r="C7" s="14" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.15">

</xml_diff>